<commit_message>
- Se agregaron Casos de Prueba
</commit_message>
<xml_diff>
--- a/Documentacion/Seguimiento/Registro de Metricas.xlsx
+++ b/Documentacion/Seguimiento/Registro de Metricas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Velocidad" sheetId="1" r:id="rId1"/>
@@ -171,13 +171,34 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -189,20 +210,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -212,14 +219,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -706,12 +706,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="1072796752"/>
-        <c:axId val="1072784240"/>
+        <c:axId val="1872214032"/>
+        <c:axId val="1872215664"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1072796752"/>
+        <c:axId val="1872214032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +748,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1072784240"/>
+        <c:crossAx val="1872215664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1072784240"/>
+        <c:axId val="1872215664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,7 +807,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1072796752"/>
+        <c:crossAx val="1872214032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1407,7 +1407,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1634,12 +1633,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="1189093616"/>
-        <c:axId val="1189089264"/>
+        <c:axId val="2056674832"/>
+        <c:axId val="2056666128"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1189093616"/>
+        <c:axId val="2056674832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1676,7 +1675,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1189089264"/>
+        <c:crossAx val="2056666128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1684,7 +1683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1189089264"/>
+        <c:axId val="2056666128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,7 +1734,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1189093616"/>
+        <c:crossAx val="2056674832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1753,7 +1752,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1865,7 +1863,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2209,7 +2206,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2458,16 +2454,16 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2543,12 +2539,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="820586592"/>
-        <c:axId val="820587136"/>
+        <c:axId val="2056670480"/>
+        <c:axId val="2056662864"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="820586592"/>
+        <c:axId val="2056670480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2585,7 +2581,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="820587136"/>
+        <c:crossAx val="2056662864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2593,7 +2589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="820587136"/>
+        <c:axId val="2056662864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2644,7 +2640,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="820586592"/>
+        <c:crossAx val="2056670480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2953,16 +2949,16 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7129,7 +7125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -7141,105 +7137,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="8">
         <v>18</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3">
+      <c r="C3" s="9"/>
+      <c r="D3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>12</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3">
+      <c r="C4" s="9"/>
+      <c r="D4" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>5</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3">
+      <c r="C5" s="9"/>
+      <c r="D5" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="8">
         <v>21</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3">
+      <c r="C6" s="9"/>
+      <c r="D6" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="8">
         <v>13</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3">
+      <c r="C7" s="9"/>
+      <c r="D7" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="8">
         <v>15</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3">
+      <c r="C8" s="9"/>
+      <c r="D8" s="1">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7258,72 +7254,72 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>168</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>111</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="8">
         <v>183</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="8">
         <v>190</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="8">
         <v>204</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="8">
         <v>196</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -7345,79 +7341,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="18"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>13</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>10</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>6</v>
+      <c r="B6" s="8">
+        <v>1</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1">
-        <v>14</v>
+      <c r="B7" s="8">
+        <v>2</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1">
-        <v>11</v>
+      <c r="B8" s="8">
+        <v>1</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1">
-        <v>12</v>
+      <c r="B9" s="8">
+        <v>4</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -7446,76 +7442,76 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="18" t="s">
+      <c r="A74" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="18" t="s">
+      <c r="A92" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="18"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="18"/>
-      <c r="H92" s="18"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="19"/>
+      <c r="H92" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>